<commit_message>
Integrate new data for bldgs/SoBRCBbG
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoBRCBbG/Shr of Blgd Rtrft Cost Borne by Govt.xlsx
+++ b/InputData/bldgs/SoBRCBbG/Shr of Blgd Rtrft Cost Borne by Govt.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\bldgs\SoBRCBbG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\bldgs\SoBRCBbG (new)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{107AC2A6-81B2-4E9B-8126-021B7368DEC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE90E8B1-C691-4CAC-90E7-E87CEDF8F5E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="75" windowWidth="24090" windowHeight="14700" xr2:uid="{B7370FBA-4486-4F99-AF7A-4FA274821588}"/>
+    <workbookView xWindow="39075" yWindow="4530" windowWidth="10590" windowHeight="15300" xr2:uid="{B7370FBA-4486-4F99-AF7A-4FA274821588}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="SoBRCBbG" sheetId="2" r:id="rId2"/>
+    <sheet name="Spending Data" sheetId="3" r:id="rId2"/>
+    <sheet name="SoBRCBbG" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>SoBRCBbG Share of Building Retrofit Costs Borne by Government</t>
   </si>
@@ -43,15 +44,6 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>U.S. Department of Energy</t>
-  </si>
-  <si>
-    <t>https://www.energystar.gov/about/federal_tax_credits/non_business_energy_property_tax_credits</t>
-  </si>
-  <si>
-    <t>Equipment Tax Credits for Primary Residences</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -61,12 +53,6 @@
     <t>under the EPS's accelerated building retrofitting policy that will be borne</t>
   </si>
   <si>
-    <t>government already pays 100% of the retrofit cost.</t>
-  </si>
-  <si>
-    <t>by the government.  It does not apply to government-owned buildings, where</t>
-  </si>
-  <si>
     <t>Unit: dimensionless (share of cost)</t>
   </si>
   <si>
@@ -80,13 +66,61 @@
   </si>
   <si>
     <t>Government Cost Share</t>
+  </si>
+  <si>
+    <t>Residential buildings</t>
+  </si>
+  <si>
+    <t>Non-residential buildings</t>
+  </si>
+  <si>
+    <t>EU spending on energy renovations (euro/year)</t>
+  </si>
+  <si>
+    <t>Public financing</t>
+  </si>
+  <si>
+    <t>Share of cost covered by public financing</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>European Commission</t>
+  </si>
+  <si>
+    <t>Accelerating energy renovation investments in buildings</t>
+  </si>
+  <si>
+    <t>https://publications.jrc.ec.europa.eu/repository/bitstream/JRC117816/accelerating_energy_renovation_investments_in_buildings.pdf</t>
+  </si>
+  <si>
+    <t>(Accessed from: https://ec.europa.eu/energy/topics/energy-efficiency/energy-efficient-buildings/financing-renovations_en)</t>
+  </si>
+  <si>
+    <t>p. 160</t>
+  </si>
+  <si>
+    <t>Table 10 (p. 29) and Table 12 (p. 32)</t>
+  </si>
+  <si>
+    <t>Comprehensive study of building energy renovation activities and the uptake of nearly zero-energy buildings in the EU</t>
+  </si>
+  <si>
+    <t>https://ec.europa.eu/energy/sites/ener/files/documents/1.final_report.pdf</t>
+  </si>
+  <si>
+    <t>by the government.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.00000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +152,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -127,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -135,12 +176,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -148,10 +199,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -463,68 +520,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01810828-2E37-43FF-9A71-F4460C03E7FB}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B4" s="2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B11" s="2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>8</v>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{E1B5812F-3104-4D2A-8EFF-45948AF0F1E7}"/>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{000A3B66-8F63-46B0-B302-00E115281537}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -532,49 +619,124 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0621FA62-16BB-4616-90B5-C4E8A6C15F77}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="41.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.73046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5">
+        <f>209326*10^6</f>
+        <v>209326000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5">
+        <f>71312*10^6</f>
+        <v>71312000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="7">
+        <f>SUM(B3:B4)</f>
+        <v>280638000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5">
+        <f>10^9</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="8">
+        <f>B7/B5</f>
+        <v>3.5633093166285391E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF72B00-B157-41C5-B107-14ECB7FAB6F3}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="1" max="1" width="39.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="B2" s="9">
+        <f>'Spending Data'!$B$9</f>
+        <v>3.5633093166285391E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9">
+        <f>'Spending Data'!$B$9</f>
+        <v>3.5633093166285391E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <v>0.1</v>
+        <v>8</v>
+      </c>
+      <c r="B4" s="9">
+        <f>'Spending Data'!$B$9</f>
+        <v>3.5633093166285391E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EU28 to EU27 variables updates bldgs/BDEQ, bldgs/DSCF, bldgs/SoBRCBbG, bldgs/SYDEC
</commit_message>
<xml_diff>
--- a/InputData/bldgs/SoBRCBbG/Shr of Blgd Rtrft Cost Borne by Govt.xlsx
+++ b/InputData/bldgs/SoBRCBbG/Shr of Blgd Rtrft Cost Borne by Govt.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\bldgs\SoBRCBbG (new)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shelley\Dropbox (Energy Innovation)\PC (2)\Documents\GitHub_Repositories\eps-eu\InputData\bldgs\SoBRCBbG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE90E8B1-C691-4CAC-90E7-E87CEDF8F5E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5EE09E-14FF-4573-829F-15F650E46C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39075" yWindow="4530" windowWidth="10590" windowHeight="15300" xr2:uid="{B7370FBA-4486-4F99-AF7A-4FA274821588}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{B7370FBA-4486-4F99-AF7A-4FA274821588}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Spending Data" sheetId="3" r:id="rId2"/>
-    <sheet name="SoBRCBbG" sheetId="2" r:id="rId3"/>
+    <sheet name="Public Financing" sheetId="4" r:id="rId3"/>
+    <sheet name="Crosswalk" sheetId="5" r:id="rId4"/>
+    <sheet name="SoBRCBbG" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
   <si>
     <t>SoBRCBbG Share of Building Retrofit Costs Borne by Government</t>
   </si>
@@ -111,14 +113,172 @@
   </si>
   <si>
     <t>by the government.</t>
+  </si>
+  <si>
+    <t>units = million Euros (MM)</t>
+  </si>
+  <si>
+    <t>EU28</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Energy related: "Total"</t>
+  </si>
+  <si>
+    <t>Residential</t>
+  </si>
+  <si>
+    <t>Non-Residential</t>
+  </si>
+  <si>
+    <t>Spending Data</t>
+  </si>
+  <si>
+    <t>Public Financing</t>
+  </si>
+  <si>
+    <t>Public resources spent on average for energy renovations in buildings across the EU every year: EUR 10 billion</t>
+  </si>
+  <si>
+    <t>Percentage of EUR 10 billion spent in the following countries:</t>
+  </si>
+  <si>
+    <t>Western and Nordic countries</t>
+  </si>
+  <si>
+    <t>Central Eastern countries</t>
+  </si>
+  <si>
+    <t>Southern European countries (Italy, Spain, Portugal, Greece, Cyprus)</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Countries Crosswalk</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Categorization</t>
+  </si>
+  <si>
+    <t>Southern European</t>
+  </si>
+  <si>
+    <t>Central Eastern</t>
+  </si>
+  <si>
+    <t>Western and Nordic</t>
+  </si>
+  <si>
+    <t>Population in 2020; source: Google</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Use 2020 population data to translate EU public resource spending data from EU28 to EU27:</t>
+  </si>
+  <si>
+    <t>UK public resource spending</t>
+  </si>
+  <si>
+    <t>EU27 public resource spending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.00000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -160,15 +320,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -185,13 +363,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -203,9 +397,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
@@ -221,6 +432,236 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>370675</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>47292</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCE0CCC4-B956-5B57-6869-11B687D8B133}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4483100" y="454025"/>
+          <a:ext cx="6403175" cy="2669842"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>373851</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>31132</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B01F3F29-D902-B426-390D-557399C9156E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4495800" y="3048000"/>
+          <a:ext cx="6393651" cy="4946032"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>469057</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>164518</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC501DE2-8761-70C9-4178-7FFA7D179443}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10820400" y="28575"/>
+          <a:ext cx="6742857" cy="4657143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>478581</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>75869</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAA70929-EF51-94E1-FFC3-177967989A14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10820400" y="4667250"/>
+          <a:ext cx="6755556" cy="2647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>73025</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>497737</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>40514</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC5C3166-DA09-C1D5-34F1-E413C9C0F3DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7045325" y="104775"/>
+          <a:ext cx="5911112" cy="6088889"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -520,18 +961,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01810828-2E37-43FF-9A71-F4460C03E7FB}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -539,79 +982,89 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B11" s="2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" s="2">
         <v>2019</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B13" s="3" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B16" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{000A3B66-8F63-46B0-B302-00E115281537}"/>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{000A3B66-8F63-46B0-B302-00E115281537}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -620,75 +1073,636 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0621FA62-16BB-4616-90B5-C4E8A6C15F77}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="5">
-        <f>209326*10^6</f>
-        <v>209326000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <f>(F49-F50)*10^6</f>
+        <v>181179000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="5">
-        <f>71312*10^6</f>
-        <v>71312000000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <f>(F54-F55)*10^6</f>
+        <v>63996000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="7">
         <f>SUM(B3:B4)</f>
-        <v>280638000000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>245175000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="5">
-        <f>10^9</f>
-        <v>1000000000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <f>'Public Financing'!C23</f>
+        <v>8415862013.6159191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="8">
         <f>B7/B5</f>
-        <v>3.5633093166285391E-3</v>
+        <v>3.4325938670810317E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E47" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49">
+        <f>209326</f>
+        <v>209326</v>
+      </c>
+    </row>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E50" t="s">
+        <v>27</v>
+      </c>
+      <c r="F50">
+        <f>28147</f>
+        <v>28147</v>
+      </c>
+    </row>
+    <row r="52" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E52" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="F53" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="54" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54">
+        <f>71312</f>
+        <v>71312</v>
+      </c>
+    </row>
+    <row r="55" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E55" t="s">
+        <v>27</v>
+      </c>
+      <c r="F55">
+        <f>7316</f>
+        <v>7316</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BBF75D-B2E5-4997-BC6C-2D3CAAE4DD17}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="26.81640625" customWidth="1"/>
+    <col min="3" max="3" width="29.7265625" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="9.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B2" s="11">
+        <f>10000000000</f>
+        <v>10000000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="12">
+        <f>0.45</f>
+        <v>0.45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="12">
+        <f>0.27</f>
+        <v>0.27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="12">
+        <f>0.28</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="13">
+        <f>SUM(B4:B6)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="5">
+        <f>1000000</f>
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="5">
+        <f>11.56*F9</f>
+        <v>11560000</v>
+      </c>
+      <c r="D10" s="20">
+        <f>C10/$C$19</f>
+        <v>6.0539638079275239E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="5">
+        <f>5.831*F9</f>
+        <v>5831000</v>
+      </c>
+      <c r="D11" s="20">
+        <f t="shared" ref="D11:D18" si="0">C11/$C$19</f>
+        <v>3.0536905678222658E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="5">
+        <f>5.531*F9</f>
+        <v>5531000</v>
+      </c>
+      <c r="D12" s="20">
+        <f t="shared" si="0"/>
+        <v>2.8965807804193024E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="5">
+        <f>67.39*F9</f>
+        <v>67390000</v>
+      </c>
+      <c r="D13" s="20">
+        <f t="shared" si="0"/>
+        <v>0.35292095243619021</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="5">
+        <f>4.995*F9</f>
+        <v>4995000</v>
+      </c>
+      <c r="D14" s="20">
+        <f t="shared" si="0"/>
+        <v>2.6158779602593413E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="5">
+        <f>0.632275*F9</f>
+        <v>632275</v>
+      </c>
+      <c r="D15" s="20">
+        <f t="shared" si="0"/>
+        <v>3.3112196943402899E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="5">
+        <f>17.44*F9</f>
+        <v>17440000</v>
+      </c>
+      <c r="D16" s="20">
+        <f t="shared" si="0"/>
+        <v>9.1333156410256078E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="5">
+        <f>10.35*F9</f>
+        <v>10350000</v>
+      </c>
+      <c r="D17" s="20">
+        <f t="shared" si="0"/>
+        <v>5.4202876654022382E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="5">
+        <f>67.22*F9</f>
+        <v>67220000</v>
+      </c>
+      <c r="D18" s="20">
+        <f t="shared" si="0"/>
+        <v>0.35203066364090674</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="5">
+        <f>SUM(C10:C18)</f>
+        <v>190949275</v>
+      </c>
+      <c r="D19" s="21">
+        <f>SUM(D10:D18)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="11">
+        <f>B2*B4*D18</f>
+        <v>1584137986.3840804</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="5">
+        <f>B2-C22</f>
+        <v>8415862013.6159191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C27" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02BFD7FB-93A8-40AE-8CBF-97E117E7496C}">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="17.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF72B00-B157-41C5-B107-14ECB7FAB6F3}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
@@ -696,15 +1710,15 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.265625" customWidth="1"/>
+    <col min="1" max="1" width="39.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -712,31 +1726,31 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="9">
         <f>'Spending Data'!$B$9</f>
-        <v>3.5633093166285391E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>3.4325938670810317E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="9">
         <f>'Spending Data'!$B$9</f>
-        <v>3.5633093166285391E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>3.4325938670810317E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="9">
         <f>'Spending Data'!$B$9</f>
-        <v>3.5633093166285391E-3</v>
+        <v>3.4325938670810317E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>